<commit_message>
latest run with updated prices for gas & elec import
</commit_message>
<xml_diff>
--- a/data/prices.xlsx
+++ b/data/prices.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/repos/github/dataknut/octopusAPI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD7B290-1601-584E-9EE4-25B4017E8A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05940956-5999-CE4B-A0F5-ECC0CAC97F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="5880" windowWidth="23620" windowHeight="15000" xr2:uid="{3CD1E604-AF5F-914E-95AF-6F9E0F046940}"/>
+    <workbookView xWindow="2720" yWindow="11400" windowWidth="16540" windowHeight="15000" xr2:uid="{3CD1E604-AF5F-914E-95AF-6F9E0F046940}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>fuel</t>
   </si>
@@ -44,9 +44,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>elec</t>
-  </si>
-  <si>
     <t>gas</t>
   </si>
   <si>
@@ -63,6 +60,30 @@
   </si>
   <si>
     <t>dateEnd</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>updated using statement of 5th May 23</t>
+  </si>
+  <si>
+    <t>updated using statement of 5th May 23 - includes EPG</t>
+  </si>
+  <si>
+    <t>elec_imp</t>
+  </si>
+  <si>
+    <t>elec_exp</t>
+  </si>
+  <si>
+    <t>Notice 20/6/23</t>
+  </si>
+  <si>
+    <t>Notice 20/6/23 claimed this was current £ but it's not!</t>
+  </si>
+  <si>
+    <t>statement of 5th May 23</t>
   </si>
 </sst>
 </file>
@@ -415,37 +436,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42ED6263-8585-3D42-BEF5-9AD9FA26441E}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>44491</v>
@@ -457,12 +481,12 @@
         <v>0.24079999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>44491</v>
@@ -474,12 +498,12 @@
         <v>0.24010000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>44473</v>
@@ -491,12 +515,12 @@
         <v>7.1900000000000006E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>44473</v>
@@ -508,64 +532,176 @@
         <v>0.26100000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>44887</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>45107</v>
+      </c>
       <c r="E6">
-        <v>0.35060000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <f>0.4893-0.1657</f>
+        <v>0.3236</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>44887</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>45107</v>
+      </c>
       <c r="E7">
-        <v>0.37290000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.40010000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
         <v>44838</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>45107</v>
+      </c>
       <c r="E8">
-        <v>0.1031</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <f>0.119-0.0219</f>
+        <v>9.7099999999999992E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>44838</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>45107</v>
+      </c>
       <c r="E9">
-        <v>0.26840000000000003</v>
+        <v>0.2616</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45108</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <v>0.30719999999999997</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45108</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11">
+        <v>0.42013</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44887</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12">
+        <v>0.1135</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45108</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13">
+        <v>7.399E-2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45108</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14">
+        <v>0.27467999999999998</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>